<commit_message>
Add new lsa from excel
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="273">
   <si>
     <t>art</t>
   </si>
@@ -803,10 +803,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>group1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -836,6 +832,30 @@
   </si>
   <si>
     <t>예매전쟁승리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>value1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>value2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>value3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>value4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>value5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>value6</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1208,9 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1224,40 +1242,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" t="s">
         <v>260</v>
       </c>
-      <c r="B1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G1" t="s">
         <v>262</v>
       </c>
-      <c r="F1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I1" t="s">
         <v>263</v>
       </c>
-      <c r="H1" t="s">
-        <v>259</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K1" t="s">
         <v>264</v>
       </c>
-      <c r="J1" t="s">
-        <v>259</v>
-      </c>
-      <c r="K1" t="s">
-        <v>265</v>
-      </c>
       <c r="L1" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -2674,7 +2692,7 @@
         <v>3.35550986692789</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D39" s="2">
         <v>2.7917594692280501</v>
@@ -2692,7 +2710,7 @@
         <v>3.35550986692789</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J39" s="2">
         <v>2.7917594692280501</v>

</xml_diff>